<commit_message>
couple quick scoring updates
</commit_message>
<xml_diff>
--- a/scoresheets/clean/Step_2/Restrictive.xlsx
+++ b/scoresheets/clean/Step_2/Restrictive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Desktop/ALSPAC-scorekeep/scoresheets/clean/Step_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B912AF45-3E5F-0E4E-B100-6D6E120F2851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECB3D69-2890-8C45-97E9-90A4913E4194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="1360" windowWidth="38260" windowHeight="23560" xr2:uid="{CA99FF3D-3E68-0F4E-879F-E897D297827B}"/>
+    <workbookView xWindow="4840" yWindow="1280" windowWidth="43060" windowHeight="25680" xr2:uid="{CA99FF3D-3E68-0F4E-879F-E897D297827B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="166">
   <si>
     <t>raw_vars</t>
   </si>
@@ -368,12 +368,6 @@
     <t>AAN cogs present at age 18 = 1, Absent = 0</t>
   </si>
   <si>
-    <t xml:space="preserve">diet_freq_d.167 +  fat_avoidance_d.167 +  fasting_monthly.167 + maladaptive_exercise.167 == 0 ~ 0, diet_freq_d.167 +  fat_avoidance_d.167 +  fasting_monthly.167 + maladaptive_exercise.167 &gt;= 1~ 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">diet_freq_d.198 +  fat_avoidance_d.198 +  fasting_monthly.198 + maladaptive_exercise.198 &lt;= 1 ~ 0, diet_freq_d.198 +  fat_avoidance_d.198 +  fasting_monthly.198 + maladaptive_exercise.198 &gt;= 2 ~ 1 </t>
-  </si>
-  <si>
     <t>wt_valuation.222 &gt; 1~1, wt_valuation.222 &lt;=1 ~ 0</t>
   </si>
   <si>
@@ -398,40 +392,166 @@
     <t>fat_avoidance.198 &lt;=0 ~ 0, fat_avoidance.198 &gt;=1~ 1</t>
   </si>
   <si>
-    <t>diet_freq_d.222 +  fasting_monthly.216 + maladaptive_exercise.216 == 0 ~ 0, diet_freq_d.222 +  fasting_monthly.216 + maladaptive_exercise.216 &gt;= 1 ~1</t>
-  </si>
-  <si>
     <t>restrict_cogs.167 ==1 &amp; restrict_behaviors.167 ==1 ~ 1, restrict_cogs.167 == 0 | restrict_behaviors.167 == 0 ~0</t>
   </si>
   <si>
-    <t>bmiz_bestavail.168 &lt;=-1 &amp; sub_restrict.167 == 1 ~1, !is.na(sub_restrict.167) &amp; bmiz_bestavail.168 &gt;-1 ~0,  !is.na(bmiz_bestavail.168) &amp; sub_restrict.167 == 0 ~ 0</t>
-  </si>
-  <si>
-    <t>bmiz_bestavail.192 &lt;=-1 &amp; sub_restrict.198 == 1 ~1, !is.na(sub_restrict.198) &amp; bmiz_bestavail.192 &gt;-1 ~0,  !is.na(bmiz_bestavail.192) &amp; sub_restrict.198 == 0 ~ 0</t>
-  </si>
-  <si>
-    <t>bmiz_bestavail.216 &lt;=-1 &amp; sub_restrict.216 == 1 ~1, !is.na(sub_restrict.216) &amp; bmiz_bestavail.168 &gt;-1 ~0,  !is.na(bmiz_bestavail.216) &amp; sub_restrict.216 == 0 ~ 0</t>
-  </si>
-  <si>
-    <t>!is.na(sub_restrict.167) &amp; bmiz_drop.168 == 0 ~0 , sub_restrict.167 ==0  &amp; !is.na(bmiz_drop.168) ~ 0, bmiz_drop.168 == 1 &amp; sub_restrict.167 ==1 ~ 1</t>
-  </si>
-  <si>
-    <t>!is.na(sub_restrict.198) &amp; bmiz_drop.192 == 0 ~0 , sub_restrict.198 ==0  &amp; !is.na(bmiz_drop.192) ~ 0, bmiz_drop.192 == 1 &amp; sub_restrict.198 ==1 ~ 1</t>
-  </si>
-  <si>
-    <t>!is.na(sub_restrict.216) &amp; bmiz_drop.216 == 0 ~0 , sub_restrict.216 ==0  &amp; !is.na(bmiz_drop.216) ~ 0, bmiz_drop.216 == 1 &amp; sub_restrict.216 ==1 ~ 1</t>
-  </si>
-  <si>
-    <t>!is.na(sub_restrict.288) &amp; bmiz_drop.288 == 0 ~0 , sub_restrict.288 ==0  &amp; !is.na(bmiz_drop.288) ~ 0, bmiz_drop.288 == 1 &amp; sub_restrict.288 ==1 ~ 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">restrict_behaviors.216 ==1 &amp; restrict_cogs.216 == 1 ~ 1, restrict_behaviors.216 == 0 | restrict_cogs.216 == 0 ~ 0 </t>
   </si>
   <si>
     <t>restrict_cogs.288 ==1 &amp; restrict_behaviors.288 ==1 ~ 1, restrict_behaviors.288 == 0 | restrict_cogs.288 == 0 ~ 0</t>
   </si>
   <si>
-    <t>bmi_bestavail.288 &lt;=18.5 &amp; sub_restrict.288 == 1 ~1, !is.na(sub_restrict.288) &amp; bmi_bestavail.288 &gt;18.5 ~0,  !is.na(bmi_bestavail.288) &amp; sub_restrict.288 == 0 ~ 0</t>
+    <t>!is.na(sub_restrict.167) &amp; bmiz_drop.168 == 0 ~ 0 , sub_restrict.167 ==0 ~ 0, bmiz_drop.168 == 1 &amp; sub_restrict.167 ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>!is.na(sub_restrict.198) &amp; bmiz_drop.192 == 0 ~0 , sub_restrict.198 ==0  ~ 0, bmiz_drop.192 == 1 &amp; sub_restrict.198 ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>!is.na(sub_restrict.216) &amp; bmiz_drop.216 == 0 ~0 , sub_restrict.216 ==0   ~ 0, bmiz_drop.216 == 1 &amp; sub_restrict.216 ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>!is.na(sub_restrict.288) &amp; bmiz_drop.288 == 0 ~0 , sub_restrict.288 ==0  ~ 0, bmiz_drop.288 == 1 &amp; sub_restrict.288 ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>diet_freq_d.222 == 0 &amp; fasting_monthly.216 == 0 &amp; maladaptive_exercise.216 == 0 ~ 0, diet_freq_d.222 == 1 | fasting_monthly.216  == 1 | maladaptive_exercise.216 == 1 ~1</t>
+  </si>
+  <si>
+    <t>bmi_bestavail.288 &lt;=18.5 &amp; sub_restrict.288 == 1 ~1, !is.na(sub_restrict.288) &amp; bmi_bestavail.288 &gt;18.5 ~0,  sub_restrict.288 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>bmiz_bestavail.216 &lt;=-1 &amp; sub_restrict.216 == 1 ~1, !is.na(sub_restrict.216) &amp; bmiz_bestavail.168 &gt;-1 ~0,  sub_restrict.216 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>bmiz_bestavail.192 &lt;=-1 &amp; sub_restrict.198 == 1 ~1, !is.na(sub_restrict.198) &amp; bmiz_bestavail.192 &gt;-1 ~0,  sub_restrict.198 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>bmiz_bestavail.168 &lt;=-1 &amp; sub_restrict.167 == 1 ~1, !is.na(sub_restrict.167) &amp; bmiz_bestavail.168 &gt;-1 ~0, sub_restrict.167 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diet_freq_d.167==0 &amp;  fat_avoidance_d.167==0 &amp; fasting_monthly.167==0 &amp; maladaptive_exercise.167 == 0 ~ 0, diet_freq_d.167 ==1|  fat_avoidance_d.167 ==1|  fasting_monthly.167 ==1| maladaptive_exercise.167 == 1~ 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(diet_freq_d.198 +  fat_avoidance_d.198 +  fasting_monthly.198 + maladaptive_exercise.198) &lt;= 1 ~ 0, (diet_freq_d.198 +  fat_avoidance_d.198 +  fasting_monthly.198 + maladaptive_exercise.198) &gt; 1 ~ 1 </t>
+  </si>
+  <si>
+    <t>restrict_behaviors_noex.167</t>
+  </si>
+  <si>
+    <t>restrict_behaviors_noex.198</t>
+  </si>
+  <si>
+    <t>restrict_behaviors_noex.216</t>
+  </si>
+  <si>
+    <t>restrict_behaviors_noex.288</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(diet_freq_d.198 +  fat_avoidance_d.198 +  fasting_monthly.198 ) &lt;= 1 ~ 0, (diet_freq_d.198 +  fat_avoidance_d.198 +  fasting_monthly.198) &gt; 1 ~ 1 </t>
+  </si>
+  <si>
+    <t>diet_freq_d.222 == 0 &amp; fasting_monthly.216  == 0 ~ 0, diet_freq_d.222 == 1 | fasting_monthly.216  == 1 ~1</t>
+  </si>
+  <si>
+    <t>fasting_monthly.288 == 1 ~1, fasting_monthly.288 == 0 ~0</t>
+  </si>
+  <si>
+    <t>sub_restrict_noex.167</t>
+  </si>
+  <si>
+    <t>sub_restrict_noex.198</t>
+  </si>
+  <si>
+    <t>sub_restrict_noex.216</t>
+  </si>
+  <si>
+    <t>sub_restrict_noex.288</t>
+  </si>
+  <si>
+    <t>AN_noex.167</t>
+  </si>
+  <si>
+    <t>AN_noex.198</t>
+  </si>
+  <si>
+    <t>AN_noex.216</t>
+  </si>
+  <si>
+    <t>AN_noex.288</t>
+  </si>
+  <si>
+    <t>AAN_noex.167</t>
+  </si>
+  <si>
+    <t>AAN_noex.198</t>
+  </si>
+  <si>
+    <t>AAN_noex.216</t>
+  </si>
+  <si>
+    <t>AAN_noex.288</t>
+  </si>
+  <si>
+    <t>restrict_cogs.167 ==1 &amp; restrict_behaviors_noex.167 ==1 ~ 1, restrict_cogs.167 == 0 | restrict_behaviors_noex.167 == 0 ~0</t>
+  </si>
+  <si>
+    <t>restrict_behaviors_noex.198 ==1 ~ 1, !is.na(restrict_behaviors_noex.198) ~ 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restrict_behaviors_noex.216 ==1 &amp; restrict_cogs.216 == 1 ~ 1, restrict_behaviors_noex.216 == 0 | restrict_cogs.216 == 0 ~ 0 </t>
+  </si>
+  <si>
+    <t>bmiz_bestavail.168 &lt;=-1 &amp; sub_restrict_noex.167 == 1 ~1, !is.na(sub_restrict_noex.167) &amp; bmiz_bestavail.168 &gt;-1 ~0, sub_restrict_noex.167 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>bmiz_bestavail.192 &lt;=-1 &amp; sub_restrict_noex.198 == 1 ~1, !is.na(sub_restrict_noex.198) &amp; bmiz_bestavail.192 &gt;-1 ~0,  sub_restrict_noex.198 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>bmiz_bestavail.216 &lt;=-1 &amp; sub_restrict_noex.216 == 1 ~1, !is.na(sub_restrict_noex.216) &amp; bmiz_bestavail.168 &gt;-1 ~0,  sub_restrict_noex.216 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>bmi_bestavail.288 &lt;=18.5 &amp; sub_restrict_noex.288 == 1 ~1, !is.na(sub_restrict_noex.288) &amp; bmi_bestavail.288 &gt;18.5 ~0,  sub_restrict_noex.288 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>!is.na(sub_restrict_noex.167) &amp; bmiz_drop.168 == 0 ~ 0 , sub_restrict_noex.167 ==0 ~ 0, bmiz_drop.168 == 1 &amp; sub_restrict_noex.167 ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>!is.na(sub_restrict_noex.198) &amp; bmiz_drop.192 == 0 ~0 , sub_restrict_noex.198 ==0  ~ 0, bmiz_drop.192 == 1 &amp; sub_restrict_noex.198 ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>!is.na(sub_restrict_noex.216) &amp; bmiz_drop.216 == 0 ~0 , sub_restrict_noex.216 ==0   ~ 0, bmiz_drop.216 == 1 &amp; sub_restrict_noex.216 ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>!is.na(sub_restrict_noex.288) &amp; bmiz_drop.288 == 0 ~0 , sub_restrict_noex.288 ==0  ~ 0, bmiz_drop.288 == 1 &amp; sub_restrict_noex.288 ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>sub_restrict_exonly.167</t>
+  </si>
+  <si>
+    <t>sub_restrict_exonly.198</t>
+  </si>
+  <si>
+    <t>sub_restrict_exonly.216</t>
+  </si>
+  <si>
+    <t>sub_restrict_exonly.288</t>
+  </si>
+  <si>
+    <t>sub_restrict.167 == 1&amp; sub_restrict_noex.167 == 0 ~ 1, sub_restrict.167 == 1 &amp; sub_restrict_noex.167 == 1 ~ 0, sub_restrict.167 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>sub_restrict.198 == 1&amp; sub_restrict_noex.198 == 0 ~ 1, sub_restrict.198 == 1 &amp; sub_restrict_noex.198 == 1 ~ 0, sub_restrict.198 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>sub_restrict.216 == 1&amp; sub_restrict_noex.216 == 0 ~ 1, sub_restrict.216 == 1 &amp; sub_restrict_noex.216 == 1 ~ 0, sub_restrict.216 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>sub_restrict.288 == 1&amp; sub_restrict_noex.288 == 0 ~ 1, sub_restrict.288 == 1 &amp; sub_restrict_noex.288 == 1 ~ 0, sub_restrict.288 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>diet_freq_d.167==0 &amp;  fat_avoidance_d.167==0 &amp; fasting_monthly.167== 0 ~ 0, diet_freq_d.167 ==1|  fat_avoidance_d.167 ==1|  fasting_monthly.167 ==1 ~ 1</t>
+  </si>
+  <si>
+    <t>restrict_cogs.288 ==1 &amp; restrict_behaviors_noex.288 ==1 ~ 1, restrict_behaviors_noex.288 == 0 | restrict_cogs.288 == 0 ~ 0</t>
   </si>
 </sst>
 </file>
@@ -887,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AF081C-D60B-0740-8510-4277D4CD09D5}">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2056,7 +2176,7 @@
         <v>16</v>
       </c>
       <c r="K33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
@@ -2160,7 +2280,7 @@
         <v>2</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2177,7 +2297,7 @@
         <v>2</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -2213,7 +2333,7 @@
         <v>16</v>
       </c>
       <c r="K40" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2249,7 +2369,7 @@
         <v>16</v>
       </c>
       <c r="K41" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -2285,7 +2405,7 @@
         <v>16</v>
       </c>
       <c r="K42" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -2325,419 +2445,1053 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A11:A14)</f>
+        <v>bmiz_drop.168,bmiz_bestavail.192,diet_freq.198,fasting_monthly.198</v>
+      </c>
       <c r="B44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G44" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" t="s">
+        <v>16</v>
+      </c>
+      <c r="J44" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A17:A20)</f>
+        <v>bmiz_drop.192,bmiz_bestavail.216,wt_valuation.222,diet_freq.222</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>54</v>
+      </c>
+      <c r="G45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A24,A25:A26)</f>
+        <v>bmi_bestavail.288,fear_wtgain.288,body_sat.288</v>
+      </c>
+      <c r="B46" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" t="s">
+        <v>16</v>
+      </c>
+      <c r="J46" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A32:A33)</f>
+        <v>fear_wtgain.167,wt_shape_concern.167,body_sat_mean.167,wt_valuation.222</v>
+      </c>
+      <c r="B47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>58</v>
+      </c>
+      <c r="G47" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48" t="s">
+        <v>60</v>
+      </c>
+      <c r="G48" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" t="s">
+        <v>16</v>
+      </c>
+      <c r="I48" t="s">
+        <v>16</v>
+      </c>
+      <c r="J48" t="s">
+        <v>16</v>
+      </c>
+      <c r="K48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
+        <v>61</v>
+      </c>
+      <c r="G49" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" t="s">
+        <v>16</v>
+      </c>
+      <c r="J49" t="s">
+        <v>16</v>
+      </c>
+      <c r="K49" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
         <v>107</v>
       </c>
-      <c r="C44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44">
+      <c r="C50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50">
         <v>4</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F50" t="s">
+        <v>62</v>
+      </c>
+      <c r="G50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" t="s">
+        <v>16</v>
+      </c>
+      <c r="J50" t="s">
+        <v>16</v>
+      </c>
+      <c r="K50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51" t="s">
+        <v>63</v>
+      </c>
+      <c r="G51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" t="s">
+        <v>16</v>
+      </c>
+      <c r="K51" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52"/>
+      <c r="B52" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52" t="s">
         <v>60</v>
       </c>
-      <c r="G44" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" t="s">
-        <v>16</v>
-      </c>
-      <c r="I44" t="s">
-        <v>16</v>
-      </c>
-      <c r="J44" t="s">
-        <v>16</v>
-      </c>
-      <c r="K44" t="s">
+      <c r="G52" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" t="s">
+        <v>16</v>
+      </c>
+      <c r="J52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53"/>
+      <c r="B53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53" t="s">
+        <v>16</v>
+      </c>
+      <c r="K53" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54"/>
+      <c r="B54" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54" t="s">
+        <v>62</v>
+      </c>
+      <c r="G54" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" t="s">
+        <v>16</v>
+      </c>
+      <c r="K54" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55"/>
+      <c r="B55" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55" t="s">
+        <v>63</v>
+      </c>
+      <c r="G55" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55" t="s">
+        <v>16</v>
+      </c>
+      <c r="K55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56"/>
+      <c r="B56" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56"/>
+      <c r="D56" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56">
+        <v>5</v>
+      </c>
+      <c r="F56"/>
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57"/>
+      <c r="B57" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57"/>
+      <c r="D57" t="s">
+        <v>20</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57"/>
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58"/>
+      <c r="B58" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58">
+        <v>5</v>
+      </c>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59"/>
+      <c r="B59" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59">
+        <v>5</v>
+      </c>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="5">
+        <v>5</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E61" s="5">
+        <v>5</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" s="5">
+        <v>5</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63" s="5">
+        <v>5</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A15,B36:B44)</f>
+        <v>fat_avoidance.198,diet_freq_d.198,diet_freq_d.222,fat_avoidance_d.167,fat_avoidance_d.198,restrict_behaviors.167,restrict_behaviors.198,restrict_behaviors.216,restrict_behaviors.288,restrict_behaviors_noex.167</v>
+      </c>
+      <c r="B64" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+      <c r="F64" t="s">
+        <v>49</v>
+      </c>
+      <c r="G64" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" t="s">
+        <v>16</v>
+      </c>
+      <c r="J64" t="s">
+        <v>16</v>
+      </c>
+      <c r="K64" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45">
-        <v>4</v>
-      </c>
-      <c r="F45" t="s">
-        <v>61</v>
-      </c>
-      <c r="G45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" t="s">
-        <v>16</v>
-      </c>
-      <c r="J45" t="s">
-        <v>16</v>
-      </c>
-      <c r="K45" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" t="s">
-        <v>20</v>
-      </c>
-      <c r="E46">
-        <v>4</v>
-      </c>
-      <c r="F46" t="s">
-        <v>62</v>
-      </c>
-      <c r="G46" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" t="s">
-        <v>16</v>
-      </c>
-      <c r="J46" t="s">
-        <v>16</v>
-      </c>
-      <c r="K46" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47">
-        <v>4</v>
-      </c>
-      <c r="F47" t="s">
-        <v>63</v>
-      </c>
-      <c r="G47" t="s">
-        <v>16</v>
-      </c>
-      <c r="H47" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" t="s">
-        <v>16</v>
-      </c>
-      <c r="K47" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="5" t="s">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,B45,A21)</f>
+        <v>restrict_behaviors_noex.198,fasting_monthly.216</v>
+      </c>
+      <c r="B65" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65" t="s">
+        <v>16</v>
+      </c>
+      <c r="D65" t="s">
+        <v>20</v>
+      </c>
+      <c r="E65">
+        <v>5</v>
+      </c>
+      <c r="F65" t="s">
+        <v>50</v>
+      </c>
+      <c r="G65" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" t="s">
+        <v>16</v>
+      </c>
+      <c r="I65" t="s">
+        <v>16</v>
+      </c>
+      <c r="J65" t="s">
+        <v>16</v>
+      </c>
+      <c r="K65" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,B46,A27,A23)</f>
+        <v>restrict_behaviors_noex.216,feel_fat.288,bmiz_drop.216</v>
+      </c>
+      <c r="B66" t="s">
+        <v>98</v>
+      </c>
+      <c r="C66" t="s">
+        <v>16</v>
+      </c>
+      <c r="D66" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66">
+        <v>5</v>
+      </c>
+      <c r="F66" t="s">
+        <v>51</v>
+      </c>
+      <c r="G66" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" t="s">
+        <v>16</v>
+      </c>
+      <c r="J66" t="s">
+        <v>16</v>
+      </c>
+      <c r="K66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A34,B38,B47)</f>
+        <v>fear_wtgain.288,body_sat.288,feel_fat.288,fat_avoidance_d.167,restrict_behaviors_noex.288</v>
+      </c>
+      <c r="B67" t="s">
+        <v>99</v>
+      </c>
+      <c r="C67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67">
+        <v>5</v>
+      </c>
+      <c r="F67" t="s">
+        <v>59</v>
+      </c>
+      <c r="G67" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" t="s">
+        <v>16</v>
+      </c>
+      <c r="J67" t="s">
+        <v>16</v>
+      </c>
+      <c r="K67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" s="5">
+      <c r="D68" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" s="5">
         <v>5</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F68" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K48" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" s="5" t="s">
+      <c r="G68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" s="5">
+      <c r="D69" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E69" s="5">
         <v>5</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F69" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K49" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C50" s="5" t="s">
+      <c r="G69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50" s="5">
+      <c r="D70" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E70" s="5">
         <v>5</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F70" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G50" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C51" s="5" t="s">
+      <c r="G70" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K70" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="5">
+      <c r="D71" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" s="5">
         <v>5</v>
       </c>
-      <c r="F51" s="5" t="s">
+      <c r="F71" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G51" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K51" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,A11,B32:B40)</f>
-        <v>bmiz_drop.168,restrict_cogs.167,restrict_cogs.216,restrict_cogs.288,diet_freq_d.167,diet_freq_d.198,diet_freq_d.222,fat_avoidance_d.167,fat_avoidance_d.198,restrict_behaviors.167</v>
-      </c>
-      <c r="B52" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52">
+      <c r="G71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K71" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A28,B49:B61)</f>
+        <v>fasting_monthly.288,sub_restrict.198,sub_restrict.216,sub_restrict.288,sub_restrict_noex.167,sub_restrict_noex.198,sub_restrict_noex.216,sub_restrict_noex.288,sub_restrict_exonly.167,sub_restrict_exonly.198,sub_restrict_exonly.216,sub_restrict_exonly.288,AN.167,AN.198</v>
+      </c>
+      <c r="B72" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72">
         <v>5</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F72" t="s">
         <v>49</v>
       </c>
-      <c r="G52" t="s">
-        <v>16</v>
-      </c>
-      <c r="H52" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" t="s">
-        <v>16</v>
-      </c>
-      <c r="J52" t="s">
-        <v>16</v>
-      </c>
-      <c r="K52" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,B41,A17)</f>
-        <v>restrict_behaviors.198,bmiz_drop.192</v>
-      </c>
-      <c r="B53" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" t="s">
-        <v>16</v>
-      </c>
-      <c r="D53" t="s">
-        <v>20</v>
-      </c>
-      <c r="E53">
+      <c r="G72" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" t="s">
+        <v>16</v>
+      </c>
+      <c r="J72" t="s">
+        <v>16</v>
+      </c>
+      <c r="K72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,B62,A34)</f>
+        <v>AN.216,fear_wtgain.288,body_sat.288,feel_fat.288</v>
+      </c>
+      <c r="B73" t="s">
+        <v>142</v>
+      </c>
+      <c r="C73" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" t="s">
+        <v>20</v>
+      </c>
+      <c r="E73">
         <v>5</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F73" t="s">
         <v>50</v>
       </c>
-      <c r="G53" t="s">
-        <v>16</v>
-      </c>
-      <c r="H53" t="s">
-        <v>16</v>
-      </c>
-      <c r="I53" t="s">
-        <v>16</v>
-      </c>
-      <c r="J53" t="s">
-        <v>16</v>
-      </c>
-      <c r="K53" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,B42,A23,A19)</f>
-        <v>restrict_behaviors.216,bmiz_drop.216,wt_valuation.222</v>
-      </c>
-      <c r="B54" t="s">
-        <v>98</v>
-      </c>
-      <c r="C54" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" t="s">
-        <v>20</v>
-      </c>
-      <c r="E54">
+      <c r="G73" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" t="s">
+        <v>16</v>
+      </c>
+      <c r="J73" t="s">
+        <v>16</v>
+      </c>
+      <c r="K73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,B63,A40,A36)</f>
+        <v>AN.288,diet_freq.167,fat_avoidance.167,fasting_monthly.167,maladaptive_exercise.167</v>
+      </c>
+      <c r="B74" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74">
         <v>5</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F74" t="s">
         <v>51</v>
       </c>
-      <c r="G54" t="s">
-        <v>16</v>
-      </c>
-      <c r="H54" t="s">
-        <v>16</v>
-      </c>
-      <c r="I54" t="s">
-        <v>16</v>
-      </c>
-      <c r="J54" t="s">
-        <v>16</v>
-      </c>
-      <c r="K54" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,A30,B34,B43)</f>
-        <v>bmiz_drop.288,restrict_cogs.288,restrict_behaviors.288</v>
-      </c>
-      <c r="B55" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" t="s">
-        <v>20</v>
-      </c>
-      <c r="E55">
+      <c r="G74" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" t="s">
+        <v>16</v>
+      </c>
+      <c r="K74" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>144</v>
+      </c>
+      <c r="C75" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" t="s">
+        <v>20</v>
+      </c>
+      <c r="E75">
         <v>5</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F75" t="s">
         <v>59</v>
       </c>
-      <c r="G55" t="s">
-        <v>16</v>
-      </c>
-      <c r="H55" t="s">
-        <v>16</v>
-      </c>
-      <c r="I55" t="s">
-        <v>16</v>
-      </c>
-      <c r="J55" t="s">
-        <v>16</v>
-      </c>
-      <c r="K55" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" t="str">
-        <f>_xlfn.TEXTJOIN(",", TRUE, A2,
- B32:B55)</f>
-        <v>id,restrict_cogs.167,restrict_cogs.216,restrict_cogs.288,diet_freq_d.167,diet_freq_d.198,diet_freq_d.222,fat_avoidance_d.167,fat_avoidance_d.198,restrict_behaviors.167,restrict_behaviors.198,restrict_behaviors.216,restrict_behaviors.288,sub_restrict.167,sub_restrict.198,sub_restrict.216,sub_restrict.288,AN.167,AN.198,AN.216,AN.288,AAN.167,AAN.198,AAN.216,AAN.288</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="G75" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" t="s">
+        <v>16</v>
+      </c>
+      <c r="I75" t="s">
+        <v>16</v>
+      </c>
+      <c r="J75" t="s">
+        <v>16</v>
+      </c>
+      <c r="K75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" t="str">
+        <f>_xlfn.TEXTJOIN(",", TRUE, A2,B32:B75)</f>
+        <v>id,restrict_cogs.167,restrict_cogs.216,restrict_cogs.288,diet_freq_d.167,diet_freq_d.198,diet_freq_d.222,fat_avoidance_d.167,fat_avoidance_d.198,restrict_behaviors.167,restrict_behaviors.198,restrict_behaviors.216,restrict_behaviors.288,restrict_behaviors_noex.167,restrict_behaviors_noex.198,restrict_behaviors_noex.216,restrict_behaviors_noex.288,sub_restrict.167,sub_restrict.198,sub_restrict.216,sub_restrict.288,sub_restrict_noex.167,sub_restrict_noex.198,sub_restrict_noex.216,sub_restrict_noex.288,sub_restrict_exonly.167,sub_restrict_exonly.198,sub_restrict_exonly.216,sub_restrict_exonly.288,AN.167,AN.198,AN.216,AN.288,AAN.167,AAN.198,AAN.216,AAN.288,AN_noex.167,AN_noex.198,AN_noex.216,AN_noex.288,AAN_noex.167,AAN_noex.198,AAN_noex.216,AAN_noex.288</v>
+      </c>
+      <c r="D76" t="s">
         <v>27</v>
       </c>
-      <c r="E56">
+      <c r="E76">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K80">
+    <sortCondition ref="E33:E80"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated for BMIZ missing restrict
</commit_message>
<xml_diff>
--- a/scoresheets/clean/Step_2/Restrictive.xlsx
+++ b/scoresheets/clean/Step_2/Restrictive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kschaumberg/Desktop/ALSPAC-scorekeep/scoresheets/clean/Step_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECB3D69-2890-8C45-97E9-90A4913E4194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD82E06-A42F-4F45-9D38-DA0409D03F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="1280" windowWidth="43060" windowHeight="25680" xr2:uid="{CA99FF3D-3E68-0F4E-879F-E897D297827B}"/>
+    <workbookView xWindow="4840" yWindow="1280" windowWidth="47880" windowHeight="25680" xr2:uid="{CA99FF3D-3E68-0F4E-879F-E897D297827B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="175">
   <si>
     <t>raw_vars</t>
   </si>
@@ -552,6 +552,33 @@
   </si>
   <si>
     <t>restrict_cogs.288 ==1 &amp; restrict_behaviors_noex.288 ==1 ~ 1, restrict_behaviors_noex.288 == 0 | restrict_cogs.288 == 0 ~ 0</t>
+  </si>
+  <si>
+    <t>Restriction with missing weight data =1, else = 0</t>
+  </si>
+  <si>
+    <t>restrict_missingwt_noex.167</t>
+  </si>
+  <si>
+    <t>restrict_missingwt_noex.198</t>
+  </si>
+  <si>
+    <t>restrict_missingwt_noex.216</t>
+  </si>
+  <si>
+    <t>restrict_missingwt_noex.288</t>
+  </si>
+  <si>
+    <t>sub_restrict_noex.198 == 1 &amp; is.na(bmiz_bestavail.192) ~ 1, sub_restrict_noex.198 == 1 &amp; is.na(bmiz_drop.192) ~ 1, sub_restrict_noex.167 == 0 ~ 0, sub_restrict_noex.198 == 1 &amp; !is.na(bmiz_bestavail.192) &amp; !is.na(bmiz_drop.192) ~ 0</t>
+  </si>
+  <si>
+    <t>sub_restrict_noex.167 == 1 &amp; is.na(bmiz_bestavail.168) ~ 1, sub_restrict_noex.167 == 1 &amp; is.na(bmiz_drop.168) ~ 1, sub_restrict_noex.167 == 0 ~ 0, sub_restrict_noex.167 == 1 &amp; !is.na(bmiz_bestavail.168) &amp; !is.na(bmiz_drop.168) ~ 0</t>
+  </si>
+  <si>
+    <t>sub_restrict_noex.216 == 1 &amp; is.na(bmiz_bestavail.216) ~ 1, sub_restrict_noex.216 == 1 &amp; is.na(bmiz_drop.216) ~ 1, sub_restrict_noex.216 == 0 ~ 0, sub_restrict_noex.216 == 1 &amp; !is.na(bmiz_bestavail.216) &amp; !is.na(bmiz_drop.216) ~ 0</t>
+  </si>
+  <si>
+    <t>sub_restrict_noex.288 == 1 &amp; is.na(bmi_bestavail.288) ~ 1, sub_restrict_noex.288 == 1 &amp; is.na(bmiz_drop.288) ~ 1, sub_restrict_noex.288 == 0 ~ 0, sub_restrict_noex.288 == 1 &amp; !is.na(bmi_bestavail.288) &amp; !is.na(bmiz_drop.288) ~ 0</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AF081C-D60B-0740-8510-4277D4CD09D5}">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K79" sqref="K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3477,20 +3504,88 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" t="str">
-        <f>_xlfn.TEXTJOIN(",", TRUE, A2,B32:B75)</f>
-        <v>id,restrict_cogs.167,restrict_cogs.216,restrict_cogs.288,diet_freq_d.167,diet_freq_d.198,diet_freq_d.222,fat_avoidance_d.167,fat_avoidance_d.198,restrict_behaviors.167,restrict_behaviors.198,restrict_behaviors.216,restrict_behaviors.288,restrict_behaviors_noex.167,restrict_behaviors_noex.198,restrict_behaviors_noex.216,restrict_behaviors_noex.288,sub_restrict.167,sub_restrict.198,sub_restrict.216,sub_restrict.288,sub_restrict_noex.167,sub_restrict_noex.198,sub_restrict_noex.216,sub_restrict_noex.288,sub_restrict_exonly.167,sub_restrict_exonly.198,sub_restrict_exonly.216,sub_restrict_exonly.288,AN.167,AN.198,AN.216,AN.288,AAN.167,AAN.198,AAN.216,AAN.288,AN_noex.167,AN_noex.198,AN_noex.216,AN_noex.288,AAN_noex.167,AAN_noex.198,AAN_noex.216,AAN_noex.288</v>
+      <c r="B76" t="s">
+        <v>167</v>
       </c>
       <c r="D76" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76">
+        <v>5</v>
+      </c>
+      <c r="F76" t="s">
+        <v>166</v>
+      </c>
+      <c r="K76" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>168</v>
+      </c>
+      <c r="D77" t="s">
+        <v>20</v>
+      </c>
+      <c r="E77">
+        <v>5</v>
+      </c>
+      <c r="F77" t="s">
+        <v>166</v>
+      </c>
+      <c r="K77" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>169</v>
+      </c>
+      <c r="D78" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78">
+        <v>5</v>
+      </c>
+      <c r="F78" t="s">
+        <v>166</v>
+      </c>
+      <c r="K78" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>170</v>
+      </c>
+      <c r="D79" t="s">
+        <v>20</v>
+      </c>
+      <c r="E79">
+        <v>5</v>
+      </c>
+      <c r="F79" t="s">
+        <v>166</v>
+      </c>
+      <c r="K79" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" t="str">
+        <f>_xlfn.TEXTJOIN(",", TRUE, A2,B32:B79)</f>
+        <v>id,restrict_cogs.167,restrict_cogs.216,restrict_cogs.288,diet_freq_d.167,diet_freq_d.198,diet_freq_d.222,fat_avoidance_d.167,fat_avoidance_d.198,restrict_behaviors.167,restrict_behaviors.198,restrict_behaviors.216,restrict_behaviors.288,restrict_behaviors_noex.167,restrict_behaviors_noex.198,restrict_behaviors_noex.216,restrict_behaviors_noex.288,sub_restrict.167,sub_restrict.198,sub_restrict.216,sub_restrict.288,sub_restrict_noex.167,sub_restrict_noex.198,sub_restrict_noex.216,sub_restrict_noex.288,sub_restrict_exonly.167,sub_restrict_exonly.198,sub_restrict_exonly.216,sub_restrict_exonly.288,AN.167,AN.198,AN.216,AN.288,AAN.167,AAN.198,AAN.216,AAN.288,AN_noex.167,AN_noex.198,AN_noex.216,AN_noex.288,AAN_noex.167,AAN_noex.198,AAN_noex.216,AAN_noex.288,restrict_missingwt_noex.167,restrict_missingwt_noex.198,restrict_missingwt_noex.216,restrict_missingwt_noex.288</v>
+      </c>
+      <c r="D80" t="s">
         <v>27</v>
       </c>
-      <c r="E76">
+      <c r="E80">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K80">
-    <sortCondition ref="E33:E80"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K84">
+    <sortCondition ref="E33:E84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>